<commit_message>
Code from Apr 23
</commit_message>
<xml_diff>
--- a/instructor/py/EDA Python Lessons/Pandas/mortality_wide.xlsx
+++ b/instructor/py/EDA Python Lessons/Pandas/mortality_wide.xlsx
@@ -465,16 +465,16 @@
         <v>1900</v>
       </c>
       <c r="B2" t="n">
-        <v>0.019838</v>
+        <v>1983.8</v>
       </c>
       <c r="C2" t="n">
-        <v>0.002983</v>
+        <v>298.3</v>
       </c>
       <c r="D2" t="n">
-        <v>0.004848</v>
+        <v>484.8</v>
       </c>
       <c r="E2" t="n">
-        <v>0.004661</v>
+        <v>466.1</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +482,16 @@
         <v>1901</v>
       </c>
       <c r="B3" t="n">
-        <v>0.01695</v>
+        <v>1695</v>
       </c>
       <c r="C3" t="n">
-        <v>0.002736</v>
+        <v>273.6</v>
       </c>
       <c r="D3" t="n">
-        <v>0.004543999999999999</v>
+        <v>454.4</v>
       </c>
       <c r="E3" t="n">
-        <v>0.004276</v>
+        <v>427.6</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +499,16 @@
         <v>1902</v>
       </c>
       <c r="B4" t="n">
-        <v>0.016557</v>
+        <v>1655.7</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002525</v>
+        <v>252.5</v>
       </c>
       <c r="D4" t="n">
-        <v>0.004215</v>
+        <v>421.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.004033</v>
+        <v>403.3</v>
       </c>
     </row>
     <row r="5">
@@ -516,16 +516,16 @@
         <v>1903</v>
       </c>
       <c r="B5" t="n">
-        <v>0.015421</v>
+        <v>1542.1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.002682</v>
+        <v>268.2</v>
       </c>
       <c r="D5" t="n">
-        <v>0.004341</v>
+        <v>434.1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.004147</v>
+        <v>414.7</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
         <v>1904</v>
       </c>
       <c r="B6" t="n">
-        <v>0.015915</v>
+        <v>1591.5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.003052</v>
+        <v>305.2</v>
       </c>
       <c r="D6" t="n">
-        <v>0.004713999999999999</v>
+        <v>471.4</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00425</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7">
@@ -550,16 +550,16 @@
         <v>1905</v>
       </c>
       <c r="B7" t="n">
-        <v>0.014989</v>
+        <v>1498.9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.002798</v>
+        <v>279.8</v>
       </c>
       <c r="D7" t="n">
-        <v>0.004393</v>
+        <v>439.3</v>
       </c>
       <c r="E7" t="n">
-        <v>0.003963</v>
+        <v>396.3</v>
       </c>
     </row>
     <row r="8">
@@ -567,16 +567,16 @@
         <v>1906</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0158</v>
+        <v>1580</v>
       </c>
       <c r="C8" t="n">
-        <v>0.002722</v>
+        <v>272.2</v>
       </c>
       <c r="D8" t="n">
-        <v>0.004452</v>
+        <v>445.2</v>
       </c>
       <c r="E8" t="n">
-        <v>0.003774</v>
+        <v>377.4</v>
       </c>
     </row>
     <row r="9">
@@ -584,16 +584,16 @@
         <v>1907</v>
       </c>
       <c r="B9" t="n">
-        <v>0.014683</v>
+        <v>1468.3</v>
       </c>
       <c r="C9" t="n">
-        <v>0.002658</v>
+        <v>265.8</v>
       </c>
       <c r="D9" t="n">
-        <v>0.004377</v>
+        <v>437.7</v>
       </c>
       <c r="E9" t="n">
-        <v>0.003656</v>
+        <v>365.6</v>
       </c>
     </row>
     <row r="10">
@@ -601,16 +601,16 @@
         <v>1908</v>
       </c>
       <c r="B10" t="n">
-        <v>0.013968</v>
+        <v>1396.8</v>
       </c>
       <c r="C10" t="n">
-        <v>0.002479</v>
+        <v>247.9</v>
       </c>
       <c r="D10" t="n">
-        <v>0.003977</v>
+        <v>397.7</v>
       </c>
       <c r="E10" t="n">
-        <v>0.003542</v>
+        <v>354.2</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +618,16 @@
         <v>1909</v>
       </c>
       <c r="B11" t="n">
-        <v>0.013489</v>
+        <v>1348.9</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002305</v>
+        <v>230.5</v>
       </c>
       <c r="D11" t="n">
-        <v>0.003636</v>
+        <v>363.6</v>
       </c>
       <c r="E11" t="n">
-        <v>0.003302</v>
+        <v>330.2</v>
       </c>
     </row>
     <row r="12">
@@ -635,16 +635,16 @@
         <v>1910</v>
       </c>
       <c r="B12" t="n">
-        <v>0.013973</v>
+        <v>1397.3</v>
       </c>
       <c r="C12" t="n">
-        <v>0.002359</v>
+        <v>235.9</v>
       </c>
       <c r="D12" t="n">
-        <v>0.003719</v>
+        <v>371.9</v>
       </c>
       <c r="E12" t="n">
-        <v>0.003484</v>
+        <v>348.4</v>
       </c>
     </row>
     <row r="13">
@@ -652,16 +652,16 @@
         <v>1911</v>
       </c>
       <c r="B13" t="n">
-        <v>0.01176</v>
+        <v>1176</v>
       </c>
       <c r="C13" t="n">
-        <v>0.002222</v>
+        <v>222.2</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00366</v>
+        <v>366</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0031</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14">
@@ -669,16 +669,16 @@
         <v>1912</v>
       </c>
       <c r="B14" t="n">
-        <v>0.010941</v>
+        <v>1094.1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.002022</v>
+        <v>202.2</v>
       </c>
       <c r="D14" t="n">
-        <v>0.003472</v>
+        <v>347.2</v>
       </c>
       <c r="E14" t="n">
-        <v>0.002875</v>
+        <v>287.5</v>
       </c>
     </row>
     <row r="15">
@@ -686,16 +686,16 @@
         <v>1913</v>
       </c>
       <c r="B15" t="n">
-        <v>0.011934</v>
+        <v>1193.4</v>
       </c>
       <c r="C15" t="n">
-        <v>0.002148</v>
+        <v>214.8</v>
       </c>
       <c r="D15" t="n">
-        <v>0.003603</v>
+        <v>360.3</v>
       </c>
       <c r="E15" t="n">
-        <v>0.003177</v>
+        <v>317.7</v>
       </c>
     </row>
     <row r="16">
@@ -703,16 +703,16 @@
         <v>1914</v>
       </c>
       <c r="B16" t="n">
-        <v>0.010242</v>
+        <v>1024.2</v>
       </c>
       <c r="C16" t="n">
-        <v>0.002072</v>
+        <v>207.2</v>
       </c>
       <c r="D16" t="n">
-        <v>0.003405</v>
+        <v>340.5</v>
       </c>
       <c r="E16" t="n">
-        <v>0.002916</v>
+        <v>291.6</v>
       </c>
     </row>
     <row r="17">
@@ -720,16 +720,16 @@
         <v>1915</v>
       </c>
       <c r="B17" t="n">
-        <v>0.009242</v>
+        <v>924.2</v>
       </c>
       <c r="C17" t="n">
-        <v>0.001967</v>
+        <v>196.7</v>
       </c>
       <c r="D17" t="n">
-        <v>0.003309</v>
+        <v>330.9</v>
       </c>
       <c r="E17" t="n">
-        <v>0.002606</v>
+        <v>260.6</v>
       </c>
     </row>
     <row r="18">
@@ -737,16 +737,16 @@
         <v>1916</v>
       </c>
       <c r="B18" t="n">
-        <v>0.011115</v>
+        <v>1111.5</v>
       </c>
       <c r="C18" t="n">
-        <v>0.002051</v>
+        <v>205.1</v>
       </c>
       <c r="D18" t="n">
-        <v>0.003558</v>
+        <v>355.8</v>
       </c>
       <c r="E18" t="n">
-        <v>0.002824</v>
+        <v>282.4</v>
       </c>
     </row>
     <row r="19">
@@ -754,16 +754,16 @@
         <v>1917</v>
       </c>
       <c r="B19" t="n">
-        <v>0.01066</v>
+        <v>1066</v>
       </c>
       <c r="C19" t="n">
-        <v>0.002189</v>
+        <v>218.9</v>
       </c>
       <c r="D19" t="n">
-        <v>0.003803</v>
+        <v>380.3</v>
       </c>
       <c r="E19" t="n">
-        <v>0.002907</v>
+        <v>290.7</v>
       </c>
     </row>
     <row r="20">
@@ -771,16 +771,16 @@
         <v>1918</v>
       </c>
       <c r="B20" t="n">
-        <v>0.015735</v>
+        <v>1573.5</v>
       </c>
       <c r="C20" t="n">
-        <v>0.003751</v>
+        <v>375.1</v>
       </c>
       <c r="D20" t="n">
-        <v>0.007774</v>
+        <v>777.4</v>
       </c>
       <c r="E20" t="n">
-        <v>0.004478999999999999</v>
+        <v>447.9</v>
       </c>
     </row>
     <row r="21">
@@ -788,16 +788,16 @@
         <v>1919</v>
       </c>
       <c r="B21" t="n">
-        <v>0.00928</v>
+        <v>928</v>
       </c>
       <c r="C21" t="n">
-        <v>0.002364</v>
+        <v>236.4</v>
       </c>
       <c r="D21" t="n">
-        <v>0.004385</v>
+        <v>438.5</v>
       </c>
       <c r="E21" t="n">
-        <v>0.003</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22">
@@ -805,16 +805,16 @@
         <v>1920</v>
       </c>
       <c r="B22" t="n">
-        <v>0.009872000000000001</v>
+        <v>987.2</v>
       </c>
       <c r="C22" t="n">
-        <v>0.002299</v>
+        <v>229.9</v>
       </c>
       <c r="D22" t="n">
-        <v>0.004029</v>
+        <v>402.9</v>
       </c>
       <c r="E22" t="n">
-        <v>0.002952</v>
+        <v>295.2</v>
       </c>
     </row>
     <row r="23">
@@ -822,16 +822,16 @@
         <v>1921</v>
       </c>
       <c r="B23" t="n">
-        <v>0.008012</v>
+        <v>801.2</v>
       </c>
       <c r="C23" t="n">
-        <v>0.002099</v>
+        <v>209.9</v>
       </c>
       <c r="D23" t="n">
-        <v>0.003265</v>
+        <v>326.5</v>
       </c>
       <c r="E23" t="n">
-        <v>0.002814</v>
+        <v>281.4</v>
       </c>
     </row>
     <row r="24">
@@ -839,16 +839,16 @@
         <v>1922</v>
       </c>
       <c r="B24" t="n">
-        <v>0.00742</v>
+        <v>742</v>
       </c>
       <c r="C24" t="n">
-        <v>0.001866</v>
+        <v>186.6</v>
       </c>
       <c r="D24" t="n">
-        <v>0.003196</v>
+        <v>319.6</v>
       </c>
       <c r="E24" t="n">
-        <v>0.002396</v>
+        <v>239.6</v>
       </c>
     </row>
     <row r="25">
@@ -856,16 +856,16 @@
         <v>1923</v>
       </c>
       <c r="B25" t="n">
-        <v>0.008067000000000001</v>
+        <v>806.7</v>
       </c>
       <c r="C25" t="n">
-        <v>0.001882</v>
+        <v>188.2</v>
       </c>
       <c r="D25" t="n">
-        <v>0.003258</v>
+        <v>325.8</v>
       </c>
       <c r="E25" t="n">
-        <v>0.0024</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26">
@@ -873,16 +873,16 @@
         <v>1924</v>
       </c>
       <c r="B26" t="n">
-        <v>0.006832</v>
+        <v>683.2</v>
       </c>
       <c r="C26" t="n">
-        <v>0.001798</v>
+        <v>179.8</v>
       </c>
       <c r="D26" t="n">
-        <v>0.003135</v>
+        <v>313.5</v>
       </c>
       <c r="E26" t="n">
-        <v>0.002217</v>
+        <v>221.7</v>
       </c>
     </row>
     <row r="27">
@@ -890,16 +890,16 @@
         <v>1925</v>
       </c>
       <c r="B27" t="n">
-        <v>0.00641</v>
+        <v>641</v>
       </c>
       <c r="C27" t="n">
-        <v>0.00181</v>
+        <v>181</v>
       </c>
       <c r="D27" t="n">
-        <v>0.00314</v>
+        <v>314</v>
       </c>
       <c r="E27" t="n">
-        <v>0.002115</v>
+        <v>211.5</v>
       </c>
     </row>
     <row r="28">
@@ -907,16 +907,16 @@
         <v>1926</v>
       </c>
       <c r="B28" t="n">
-        <v>0.007234</v>
+        <v>723.4</v>
       </c>
       <c r="C28" t="n">
-        <v>0.001714</v>
+        <v>171.4</v>
       </c>
       <c r="D28" t="n">
-        <v>0.003075</v>
+        <v>307.5</v>
       </c>
       <c r="E28" t="n">
-        <v>0.002138</v>
+        <v>213.8</v>
       </c>
     </row>
     <row r="29">
@@ -924,16 +924,16 @@
         <v>1927</v>
       </c>
       <c r="B29" t="n">
-        <v>0.00591</v>
+        <v>591</v>
       </c>
       <c r="C29" t="n">
-        <v>0.001675</v>
+        <v>167.5</v>
       </c>
       <c r="D29" t="n">
-        <v>0.002895</v>
+        <v>289.5</v>
       </c>
       <c r="E29" t="n">
-        <v>0.002083</v>
+        <v>208.3</v>
       </c>
     </row>
     <row r="30">
@@ -941,16 +941,16 @@
         <v>1928</v>
       </c>
       <c r="B30" t="n">
-        <v>0.006475</v>
+        <v>647.5</v>
       </c>
       <c r="C30" t="n">
-        <v>0.001738</v>
+        <v>173.8</v>
       </c>
       <c r="D30" t="n">
-        <v>0.003078</v>
+        <v>307.8</v>
       </c>
       <c r="E30" t="n">
-        <v>0.002131</v>
+        <v>213.1</v>
       </c>
     </row>
     <row r="31">
@@ -958,16 +958,16 @@
         <v>1929</v>
       </c>
       <c r="B31" t="n">
-        <v>0.006255</v>
+        <v>625.5</v>
       </c>
       <c r="C31" t="n">
-        <v>0.00165</v>
+        <v>165</v>
       </c>
       <c r="D31" t="n">
-        <v>0.00298</v>
+        <v>298</v>
       </c>
       <c r="E31" t="n">
-        <v>0.00208</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32">
@@ -975,16 +975,16 @@
         <v>1930</v>
       </c>
       <c r="B32" t="n">
-        <v>0.005636</v>
+        <v>563.6</v>
       </c>
       <c r="C32" t="n">
-        <v>0.001528</v>
+        <v>152.8</v>
       </c>
       <c r="D32" t="n">
-        <v>0.002778</v>
+        <v>277.8</v>
       </c>
       <c r="E32" t="n">
-        <v>0.001898</v>
+        <v>189.8</v>
       </c>
     </row>
     <row r="33">
@@ -992,16 +992,16 @@
         <v>1931</v>
       </c>
       <c r="B33" t="n">
-        <v>0.005266</v>
+        <v>526.6</v>
       </c>
       <c r="C33" t="n">
-        <v>0.001503</v>
+        <v>150.3</v>
       </c>
       <c r="D33" t="n">
-        <v>0.002635</v>
+        <v>263.5</v>
       </c>
       <c r="E33" t="n">
-        <v>0.00182</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34">
@@ -1009,16 +1009,16 @@
         <v>1932</v>
       </c>
       <c r="B34" t="n">
-        <v>0.004619</v>
+        <v>461.9</v>
       </c>
       <c r="C34" t="n">
-        <v>0.001422</v>
+        <v>142.2</v>
       </c>
       <c r="D34" t="n">
-        <v>0.002375</v>
+        <v>237.5</v>
       </c>
       <c r="E34" t="n">
-        <v>0.001659</v>
+        <v>165.9</v>
       </c>
     </row>
     <row r="35">
@@ -1026,16 +1026,16 @@
         <v>1933</v>
       </c>
       <c r="B35" t="n">
-        <v>0.004726</v>
+        <v>472.6</v>
       </c>
       <c r="C35" t="n">
-        <v>0.00138</v>
+        <v>138</v>
       </c>
       <c r="D35" t="n">
-        <v>0.002234</v>
+        <v>223.4</v>
       </c>
       <c r="E35" t="n">
-        <v>0.001613</v>
+        <v>161.3</v>
       </c>
     </row>
     <row r="36">
@@ -1043,16 +1043,16 @@
         <v>1934</v>
       </c>
       <c r="B36" t="n">
-        <v>0.005077</v>
+        <v>507.7</v>
       </c>
       <c r="C36" t="n">
-        <v>0.001415</v>
+        <v>141.5</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00224</v>
+        <v>224</v>
       </c>
       <c r="E36" t="n">
-        <v>0.001651</v>
+        <v>165.1</v>
       </c>
     </row>
     <row r="37">
@@ -1060,16 +1060,16 @@
         <v>1935</v>
       </c>
       <c r="B37" t="n">
-        <v>0.004409</v>
+        <v>440.9</v>
       </c>
       <c r="C37" t="n">
-        <v>0.001434</v>
+        <v>143.4</v>
       </c>
       <c r="D37" t="n">
-        <v>0.002223</v>
+        <v>222.3</v>
       </c>
       <c r="E37" t="n">
-        <v>0.001624</v>
+        <v>162.4</v>
       </c>
     </row>
     <row r="38">
@@ -1077,16 +1077,16 @@
         <v>1936</v>
       </c>
       <c r="B38" t="n">
-        <v>0.004398</v>
+        <v>439.8</v>
       </c>
       <c r="C38" t="n">
-        <v>0.00141</v>
+        <v>141</v>
       </c>
       <c r="D38" t="n">
-        <v>0.002304</v>
+        <v>230.4</v>
       </c>
       <c r="E38" t="n">
-        <v>0.001546</v>
+        <v>154.6</v>
       </c>
     </row>
     <row r="39">
@@ -1094,16 +1094,16 @@
         <v>1937</v>
       </c>
       <c r="B39" t="n">
-        <v>0.004187</v>
+        <v>418.7</v>
       </c>
       <c r="C39" t="n">
-        <v>0.001283</v>
+        <v>128.3</v>
       </c>
       <c r="D39" t="n">
-        <v>0.00219</v>
+        <v>219</v>
       </c>
       <c r="E39" t="n">
-        <v>0.001429</v>
+        <v>142.9</v>
       </c>
     </row>
     <row r="40">
@@ -1111,16 +1111,16 @@
         <v>1938</v>
       </c>
       <c r="B40" t="n">
-        <v>0.003838</v>
+        <v>383.8</v>
       </c>
       <c r="C40" t="n">
-        <v>0.001138</v>
+        <v>113.8</v>
       </c>
       <c r="D40" t="n">
-        <v>0.001923</v>
+        <v>192.3</v>
       </c>
       <c r="E40" t="n">
-        <v>0.001288</v>
+        <v>128.8</v>
       </c>
     </row>
     <row r="41">
@@ -1128,16 +1128,16 @@
         <v>1939</v>
       </c>
       <c r="B41" t="n">
-        <v>0.003183</v>
+        <v>318.3</v>
       </c>
       <c r="C41" t="n">
-        <v>0.001065</v>
+        <v>106.5</v>
       </c>
       <c r="D41" t="n">
-        <v>0.001798</v>
+        <v>179.8</v>
       </c>
       <c r="E41" t="n">
-        <v>0.001126</v>
+        <v>112.6</v>
       </c>
     </row>
     <row r="42">
@@ -1145,16 +1145,16 @@
         <v>1940</v>
       </c>
       <c r="B42" t="n">
-        <v>0.002896</v>
+        <v>289.6</v>
       </c>
       <c r="C42" t="n">
-        <v>0.000995</v>
+        <v>99.5</v>
       </c>
       <c r="D42" t="n">
-        <v>0.001716</v>
+        <v>171.6</v>
       </c>
       <c r="E42" t="n">
-        <v>0.001083</v>
+        <v>108.3</v>
       </c>
     </row>
     <row r="43">
@@ -1162,16 +1162,16 @@
         <v>1941</v>
       </c>
       <c r="B43" t="n">
-        <v>0.002799</v>
+        <v>279.9</v>
       </c>
       <c r="C43" t="n">
-        <v>0.000947</v>
+        <v>94.7</v>
       </c>
       <c r="D43" t="n">
-        <v>0.00169</v>
+        <v>169</v>
       </c>
       <c r="E43" t="n">
-        <v>0.001038</v>
+        <v>103.8</v>
       </c>
     </row>
     <row r="44">
@@ -1179,16 +1179,16 @@
         <v>1942</v>
       </c>
       <c r="B44" t="n">
-        <v>0.002434</v>
+        <v>243.4</v>
       </c>
       <c r="C44" t="n">
-        <v>0.0008579999999999999</v>
+        <v>85.8</v>
       </c>
       <c r="D44" t="n">
-        <v>0.001547</v>
+        <v>154.7</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0009609999999999999</v>
+        <v>96.09999999999999</v>
       </c>
     </row>
     <row r="45">
@@ -1196,16 +1196,16 @@
         <v>1943</v>
       </c>
       <c r="B45" t="n">
-        <v>0.002564</v>
+        <v>256.4</v>
       </c>
       <c r="C45" t="n">
-        <v>0.0009059999999999999</v>
+        <v>90.59999999999999</v>
       </c>
       <c r="D45" t="n">
-        <v>0.00164</v>
+        <v>164</v>
       </c>
       <c r="E45" t="n">
-        <v>0.001031</v>
+        <v>103.1</v>
       </c>
     </row>
     <row r="46">
@@ -1213,16 +1213,16 @@
         <v>1944</v>
       </c>
       <c r="B46" t="n">
-        <v>0.00233</v>
+        <v>233</v>
       </c>
       <c r="C46" t="n">
-        <v>0.000897</v>
+        <v>89.7</v>
       </c>
       <c r="D46" t="n">
-        <v>0.001579</v>
+        <v>157.9</v>
       </c>
       <c r="E46" t="n">
-        <v>0.000987</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="47">
@@ -1230,16 +1230,16 @@
         <v>1945</v>
       </c>
       <c r="B47" t="n">
-        <v>0.00203</v>
+        <v>203</v>
       </c>
       <c r="C47" t="n">
-        <v>0.000868</v>
+        <v>86.8</v>
       </c>
       <c r="D47" t="n">
-        <v>0.001523</v>
+        <v>152.3</v>
       </c>
       <c r="E47" t="n">
-        <v>0.000936</v>
+        <v>93.59999999999999</v>
       </c>
     </row>
     <row r="48">
@@ -1247,16 +1247,16 @@
         <v>1946</v>
       </c>
       <c r="B48" t="n">
-        <v>0.001815</v>
+        <v>181.5</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0007859999999999999</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="D48" t="n">
-        <v>0.001378</v>
+        <v>137.8</v>
       </c>
       <c r="E48" t="n">
-        <v>0.000856</v>
+        <v>85.59999999999999</v>
       </c>
     </row>
     <row r="49">
@@ -1264,16 +1264,16 @@
         <v>1947</v>
       </c>
       <c r="B49" t="n">
-        <v>0.001608</v>
+        <v>160.8</v>
       </c>
       <c r="C49" t="n">
-        <v>0.000679</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="D49" t="n">
-        <v>0.001268</v>
+        <v>126.8</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0007329999999999999</v>
+        <v>73.3</v>
       </c>
     </row>
     <row r="50">
@@ -1281,16 +1281,16 @@
         <v>1948</v>
       </c>
       <c r="B50" t="n">
-        <v>0.001601</v>
+        <v>160.1</v>
       </c>
       <c r="C50" t="n">
-        <v>0.0006559999999999999</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="D50" t="n">
-        <v>0.001187</v>
+        <v>118.7</v>
       </c>
       <c r="E50" t="n">
-        <v>0.0007059999999999999</v>
+        <v>70.59999999999999</v>
       </c>
     </row>
     <row r="51">
@@ -1298,16 +1298,16 @@
         <v>1949</v>
       </c>
       <c r="B51" t="n">
-        <v>0.001502</v>
+        <v>150.2</v>
       </c>
       <c r="C51" t="n">
-        <v>0.0006360000000000001</v>
+        <v>63.6</v>
       </c>
       <c r="D51" t="n">
-        <v>0.001118</v>
+        <v>111.8</v>
       </c>
       <c r="E51" t="n">
-        <v>0.000682</v>
+        <v>68.2</v>
       </c>
     </row>
     <row r="52">
@@ -1315,16 +1315,16 @@
         <v>1950</v>
       </c>
       <c r="B52" t="n">
-        <v>0.001394</v>
+        <v>139.4</v>
       </c>
       <c r="C52" t="n">
-        <v>0.000581</v>
+        <v>58.1</v>
       </c>
       <c r="D52" t="n">
-        <v>0.001086</v>
+        <v>108.6</v>
       </c>
       <c r="E52" t="n">
-        <v>0.000617</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="53">
@@ -1332,16 +1332,16 @@
         <v>1951</v>
       </c>
       <c r="B53" t="n">
-        <v>0.001369</v>
+        <v>136.9</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0005639999999999999</v>
+        <v>56.4</v>
       </c>
       <c r="D53" t="n">
-        <v>0.001089</v>
+        <v>108.9</v>
       </c>
       <c r="E53" t="n">
-        <v>0.000617</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="54">
@@ -1349,16 +1349,16 @@
         <v>1952</v>
       </c>
       <c r="B54" t="n">
-        <v>0.001411</v>
+        <v>141.1</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0005679999999999999</v>
+        <v>56.8</v>
       </c>
       <c r="D54" t="n">
-        <v>0.001144</v>
+        <v>114.4</v>
       </c>
       <c r="E54" t="n">
-        <v>0.0006129999999999999</v>
+        <v>61.3</v>
       </c>
     </row>
     <row r="55">
@@ -1366,16 +1366,16 @@
         <v>1953</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0013</v>
+        <v>130</v>
       </c>
       <c r="C55" t="n">
-        <v>0.000531</v>
+        <v>53.1</v>
       </c>
       <c r="D55" t="n">
-        <v>0.001069</v>
+        <v>106.9</v>
       </c>
       <c r="E55" t="n">
-        <v>0.000561</v>
+        <v>56.1</v>
       </c>
     </row>
     <row r="56">
@@ -1383,16 +1383,16 @@
         <v>1954</v>
       </c>
       <c r="B56" t="n">
-        <v>0.001183</v>
+        <v>118.3</v>
       </c>
       <c r="C56" t="n">
-        <v>0.000478</v>
+        <v>47.8</v>
       </c>
       <c r="D56" t="n">
-        <v>0.0009609999999999999</v>
+        <v>96.09999999999999</v>
       </c>
       <c r="E56" t="n">
-        <v>0.000525</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="57">
@@ -1400,16 +1400,16 @@
         <v>1955</v>
       </c>
       <c r="B57" t="n">
-        <v>0.001134</v>
+        <v>113.4</v>
       </c>
       <c r="C57" t="n">
-        <v>0.000466</v>
+        <v>46.6</v>
       </c>
       <c r="D57" t="n">
-        <v>0.000973</v>
+        <v>97.3</v>
       </c>
       <c r="E57" t="n">
-        <v>0.000506</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="58">
@@ -1417,16 +1417,16 @@
         <v>1956</v>
       </c>
       <c r="B58" t="n">
-        <v>0.001102</v>
+        <v>110.2</v>
       </c>
       <c r="C58" t="n">
-        <v>0.000463</v>
+        <v>46.3</v>
       </c>
       <c r="D58" t="n">
-        <v>0.000972</v>
+        <v>97.2</v>
       </c>
       <c r="E58" t="n">
-        <v>0.000483</v>
+        <v>48.3</v>
       </c>
     </row>
     <row r="59">
@@ -1434,16 +1434,16 @@
         <v>1957</v>
       </c>
       <c r="B59" t="n">
-        <v>0.001118</v>
+        <v>111.8</v>
       </c>
       <c r="C59" t="n">
-        <v>0.000474</v>
+        <v>47.4</v>
       </c>
       <c r="D59" t="n">
-        <v>0.001002</v>
+        <v>100.2</v>
       </c>
       <c r="E59" t="n">
-        <v>0.000501</v>
+        <v>50.1</v>
       </c>
     </row>
     <row r="60">
@@ -1451,16 +1451,16 @@
         <v>1958</v>
       </c>
       <c r="B60" t="n">
-        <v>0.001117</v>
+        <v>111.7</v>
       </c>
       <c r="C60" t="n">
-        <v>0.000446</v>
+        <v>44.6</v>
       </c>
       <c r="D60" t="n">
-        <v>0.000915</v>
+        <v>91.5</v>
       </c>
       <c r="E60" t="n">
-        <v>0.000484</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="61">
@@ -1468,16 +1468,16 @@
         <v>1959</v>
       </c>
       <c r="B61" t="n">
-        <v>0.001069</v>
+        <v>106.9</v>
       </c>
       <c r="C61" t="n">
-        <v>0.000458</v>
+        <v>45.8</v>
       </c>
       <c r="D61" t="n">
-        <v>0.000928</v>
+        <v>92.8</v>
       </c>
       <c r="E61" t="n">
-        <v>0.000494</v>
+        <v>49.4</v>
       </c>
     </row>
     <row r="62">
@@ -1485,16 +1485,16 @@
         <v>1960</v>
       </c>
       <c r="B62" t="n">
-        <v>0.001091</v>
+        <v>109.1</v>
       </c>
       <c r="C62" t="n">
-        <v>0.00044</v>
+        <v>44</v>
       </c>
       <c r="D62" t="n">
-        <v>0.0009220000000000001</v>
+        <v>92.2</v>
       </c>
       <c r="E62" t="n">
-        <v>0.00049</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63">
@@ -1502,16 +1502,16 @@
         <v>1961</v>
       </c>
       <c r="B63" t="n">
-        <v>0.001017</v>
+        <v>101.7</v>
       </c>
       <c r="C63" t="n">
-        <v>0.000419</v>
+        <v>41.9</v>
       </c>
       <c r="D63" t="n">
-        <v>0.0008809999999999999</v>
+        <v>88.09999999999999</v>
       </c>
       <c r="E63" t="n">
-        <v>0.000458</v>
+        <v>45.8</v>
       </c>
     </row>
     <row r="64">
@@ -1519,16 +1519,16 @@
         <v>1962</v>
       </c>
       <c r="B64" t="n">
-        <v>0.000992</v>
+        <v>99.2</v>
       </c>
       <c r="C64" t="n">
-        <v>0.000419</v>
+        <v>41.9</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0008759999999999999</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="E64" t="n">
-        <v>0.000456</v>
+        <v>45.6</v>
       </c>
     </row>
     <row r="65">
@@ -1536,16 +1536,16 @@
         <v>1963</v>
       </c>
       <c r="B65" t="n">
-        <v>0.001015</v>
+        <v>101.5</v>
       </c>
       <c r="C65" t="n">
-        <v>0.000412</v>
+        <v>41.2</v>
       </c>
       <c r="D65" t="n">
-        <v>0.000905</v>
+        <v>90.5</v>
       </c>
       <c r="E65" t="n">
-        <v>0.000453</v>
+        <v>45.3</v>
       </c>
     </row>
     <row r="66">
@@ -1553,16 +1553,16 @@
         <v>1964</v>
       </c>
       <c r="B66" t="n">
-        <v>0.000985</v>
+        <v>98.5</v>
       </c>
       <c r="C66" t="n">
-        <v>0.000416</v>
+        <v>41.6</v>
       </c>
       <c r="D66" t="n">
-        <v>0.0009390000000000001</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="E66" t="n">
-        <v>0.000446</v>
+        <v>44.6</v>
       </c>
     </row>
     <row r="67">
@@ -1570,16 +1570,16 @@
         <v>1965</v>
       </c>
       <c r="B67" t="n">
-        <v>0.0009590000000000001</v>
+        <v>95.90000000000001</v>
       </c>
       <c r="C67" t="n">
-        <v>0.000405</v>
+        <v>40.5</v>
       </c>
       <c r="D67" t="n">
-        <v>0.000953</v>
+        <v>95.3</v>
       </c>
       <c r="E67" t="n">
-        <v>0.000439</v>
+        <v>43.9</v>
       </c>
     </row>
     <row r="68">
@@ -1587,16 +1587,16 @@
         <v>1966</v>
       </c>
       <c r="B68" t="n">
-        <v>0.000964</v>
+        <v>96.40000000000001</v>
       </c>
       <c r="C68" t="n">
-        <v>0.000411</v>
+        <v>41.1</v>
       </c>
       <c r="D68" t="n">
-        <v>0.00102</v>
+        <v>102</v>
       </c>
       <c r="E68" t="n">
-        <v>0.000443</v>
+        <v>44.3</v>
       </c>
     </row>
     <row r="69">
@@ -1604,16 +1604,16 @@
         <v>1967</v>
       </c>
       <c r="B69" t="n">
-        <v>0.000894</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="C69" t="n">
-        <v>0.000405</v>
+        <v>40.5</v>
       </c>
       <c r="D69" t="n">
-        <v>0.001021</v>
+        <v>102.1</v>
       </c>
       <c r="E69" t="n">
-        <v>0.000429</v>
+        <v>42.9</v>
       </c>
     </row>
     <row r="70">
@@ -1621,16 +1621,16 @@
         <v>1968</v>
       </c>
       <c r="B70" t="n">
-        <v>0.000896</v>
+        <v>89.59999999999999</v>
       </c>
       <c r="C70" t="n">
-        <v>0.000416</v>
+        <v>41.6</v>
       </c>
       <c r="D70" t="n">
-        <v>0.001081</v>
+        <v>108.1</v>
       </c>
       <c r="E70" t="n">
-        <v>0.000445</v>
+        <v>44.5</v>
       </c>
     </row>
     <row r="71">
@@ -1638,16 +1638,16 @@
         <v>1969</v>
       </c>
       <c r="B71" t="n">
-        <v>0.00088</v>
+        <v>88</v>
       </c>
       <c r="C71" t="n">
-        <v>0.000413</v>
+        <v>41.3</v>
       </c>
       <c r="D71" t="n">
-        <v>0.001135</v>
+        <v>113.5</v>
       </c>
       <c r="E71" t="n">
-        <v>0.00044</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72">
@@ -1655,16 +1655,16 @@
         <v>1970</v>
       </c>
       <c r="B72" t="n">
-        <v>0.000845</v>
+        <v>84.5</v>
       </c>
       <c r="C72" t="n">
-        <v>0.000406</v>
+        <v>40.6</v>
       </c>
       <c r="D72" t="n">
-        <v>0.001103</v>
+        <v>110.3</v>
       </c>
       <c r="E72" t="n">
-        <v>0.000421</v>
+        <v>42.1</v>
       </c>
     </row>
     <row r="73">
@@ -1672,16 +1672,16 @@
         <v>1971</v>
       </c>
       <c r="B73" t="n">
-        <v>0.0008229999999999999</v>
+        <v>82.3</v>
       </c>
       <c r="C73" t="n">
-        <v>0.000399</v>
+        <v>39.9</v>
       </c>
       <c r="D73" t="n">
-        <v>0.001103</v>
+        <v>110.3</v>
       </c>
       <c r="E73" t="n">
-        <v>0.00042</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74">
@@ -1689,16 +1689,16 @@
         <v>1972</v>
       </c>
       <c r="B74" t="n">
-        <v>0.000804</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="C74" t="n">
-        <v>0.000404</v>
+        <v>40.4</v>
       </c>
       <c r="D74" t="n">
-        <v>0.001104</v>
+        <v>110.4</v>
       </c>
       <c r="E74" t="n">
-        <v>0.000408</v>
+        <v>40.8</v>
       </c>
     </row>
     <row r="75">
@@ -1706,16 +1706,16 @@
         <v>1973</v>
       </c>
       <c r="B75" t="n">
-        <v>0.00079</v>
+        <v>79</v>
       </c>
       <c r="C75" t="n">
-        <v>0.000403</v>
+        <v>40.3</v>
       </c>
       <c r="D75" t="n">
-        <v>0.00111</v>
+        <v>111</v>
       </c>
       <c r="E75" t="n">
-        <v>0.000411</v>
+        <v>41.1</v>
       </c>
     </row>
     <row r="76">
@@ -1723,16 +1723,16 @@
         <v>1974</v>
       </c>
       <c r="B76" t="n">
-        <v>0.0007329999999999999</v>
+        <v>73.3</v>
       </c>
       <c r="C76" t="n">
-        <v>0.000383</v>
+        <v>38.3</v>
       </c>
       <c r="D76" t="n">
-        <v>0.001048</v>
+        <v>104.8</v>
       </c>
       <c r="E76" t="n">
-        <v>0.000372</v>
+        <v>37.2</v>
       </c>
     </row>
     <row r="77">
@@ -1740,16 +1740,16 @@
         <v>1975</v>
       </c>
       <c r="B77" t="n">
-        <v>0.0006990000000000001</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="C77" t="n">
-        <v>0.000353</v>
+        <v>35.3</v>
       </c>
       <c r="D77" t="n">
-        <v>0.001002</v>
+        <v>100.2</v>
       </c>
       <c r="E77" t="n">
-        <v>0.000352</v>
+        <v>35.2</v>
       </c>
     </row>
     <row r="78">
@@ -1757,16 +1757,16 @@
         <v>1976</v>
       </c>
       <c r="B78" t="n">
-        <v>0.0006879999999999999</v>
+        <v>68.8</v>
       </c>
       <c r="C78" t="n">
-        <v>0.000342</v>
+        <v>34.2</v>
       </c>
       <c r="D78" t="n">
-        <v>0.0009570000000000001</v>
+        <v>95.7</v>
       </c>
       <c r="E78" t="n">
-        <v>0.000341</v>
+        <v>34.1</v>
       </c>
     </row>
     <row r="79">
@@ -1774,16 +1774,16 @@
         <v>1977</v>
       </c>
       <c r="B79" t="n">
-        <v>0.000676</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="C79" t="n">
-        <v>0.000346</v>
+        <v>34.6</v>
       </c>
       <c r="D79" t="n">
-        <v>0.000998</v>
+        <v>99.8</v>
       </c>
       <c r="E79" t="n">
-        <v>0.000333</v>
+        <v>33.3</v>
       </c>
     </row>
     <row r="80">
@@ -1791,16 +1791,16 @@
         <v>1978</v>
       </c>
       <c r="B80" t="n">
-        <v>0.000679</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="C80" t="n">
-        <v>0.000337</v>
+        <v>33.7</v>
       </c>
       <c r="D80" t="n">
-        <v>0.0009890000000000001</v>
+        <v>98.90000000000001</v>
       </c>
       <c r="E80" t="n">
-        <v>0.000327</v>
+        <v>32.7</v>
       </c>
     </row>
     <row r="81">
@@ -1808,16 +1808,16 @@
         <v>1979</v>
       </c>
       <c r="B81" t="n">
-        <v>0.000642</v>
+        <v>64.2</v>
       </c>
       <c r="C81" t="n">
-        <v>0.000318</v>
+        <v>31.8</v>
       </c>
       <c r="D81" t="n">
-        <v>0.0009879999999999999</v>
+        <v>98.8</v>
       </c>
       <c r="E81" t="n">
-        <v>0.000311</v>
+        <v>31.1</v>
       </c>
     </row>
     <row r="82">
@@ -1825,16 +1825,16 @@
         <v>1980</v>
       </c>
       <c r="B82" t="n">
-        <v>0.000639</v>
+        <v>63.9</v>
       </c>
       <c r="C82" t="n">
-        <v>0.000308</v>
+        <v>30.8</v>
       </c>
       <c r="D82" t="n">
-        <v>0.0009790000000000001</v>
+        <v>97.90000000000001</v>
       </c>
       <c r="E82" t="n">
-        <v>0.000304</v>
+        <v>30.4</v>
       </c>
     </row>
     <row r="83">
@@ -1842,16 +1842,16 @@
         <v>1981</v>
       </c>
       <c r="B83" t="n">
-        <v>0.000606</v>
+        <v>60.6</v>
       </c>
       <c r="C83" t="n">
-        <v>0.000295</v>
+        <v>29.5</v>
       </c>
       <c r="D83" t="n">
-        <v>0.0009</v>
+        <v>90</v>
       </c>
       <c r="E83" t="n">
-        <v>0.000291</v>
+        <v>29.1</v>
       </c>
     </row>
     <row r="84">
@@ -1859,16 +1859,16 @@
         <v>1982</v>
       </c>
       <c r="B84" t="n">
-        <v>0.0005820000000000001</v>
+        <v>58.2</v>
       </c>
       <c r="C84" t="n">
-        <v>0.000282</v>
+        <v>28.2</v>
       </c>
       <c r="D84" t="n">
-        <v>0.000854</v>
+        <v>85.40000000000001</v>
       </c>
       <c r="E84" t="n">
-        <v>0.000283</v>
+        <v>28.3</v>
       </c>
     </row>
     <row r="85">
@@ -1876,16 +1876,16 @@
         <v>1983</v>
       </c>
       <c r="B85" t="n">
-        <v>0.000561</v>
+        <v>56.1</v>
       </c>
       <c r="C85" t="n">
-        <v>0.000273</v>
+        <v>27.3</v>
       </c>
       <c r="D85" t="n">
-        <v>0.000811</v>
+        <v>81.09999999999999</v>
       </c>
       <c r="E85" t="n">
-        <v>0.000265</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="86">
@@ -1893,16 +1893,16 @@
         <v>1984</v>
       </c>
       <c r="B86" t="n">
-        <v>0.000522</v>
+        <v>52.2</v>
       </c>
       <c r="C86" t="n">
-        <v>0.000283</v>
+        <v>28.3</v>
       </c>
       <c r="D86" t="n">
-        <v>0.000804</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="E86" t="n">
-        <v>0.000253</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="87">
@@ -1910,16 +1910,16 @@
         <v>1985</v>
       </c>
       <c r="B87" t="n">
-        <v>0.000518</v>
+        <v>51.8</v>
       </c>
       <c r="C87" t="n">
-        <v>0.00028</v>
+        <v>28</v>
       </c>
       <c r="D87" t="n">
-        <v>0.0008050000000000001</v>
+        <v>80.5</v>
       </c>
       <c r="E87" t="n">
-        <v>0.00025</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88">
@@ -1927,16 +1927,16 @@
         <v>1986</v>
       </c>
       <c r="B88" t="n">
-        <v>0.0005239999999999999</v>
+        <v>52.4</v>
       </c>
       <c r="C88" t="n">
-        <v>0.000286</v>
+        <v>28.6</v>
       </c>
       <c r="D88" t="n">
-        <v>0.000862</v>
+        <v>86.2</v>
       </c>
       <c r="E88" t="n">
-        <v>0.000239</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="89">
@@ -1944,16 +1944,16 @@
         <v>1987</v>
       </c>
       <c r="B89" t="n">
-        <v>0.000521</v>
+        <v>52.1</v>
       </c>
       <c r="C89" t="n">
-        <v>0.000271</v>
+        <v>27.1</v>
       </c>
       <c r="D89" t="n">
-        <v>0.000835</v>
+        <v>83.5</v>
       </c>
       <c r="E89" t="n">
-        <v>0.000247</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="90">
@@ -1961,16 +1961,16 @@
         <v>1988</v>
       </c>
       <c r="B90" t="n">
-        <v>0.000515</v>
+        <v>51.5</v>
       </c>
       <c r="C90" t="n">
-        <v>0.000277</v>
+        <v>27.7</v>
       </c>
       <c r="D90" t="n">
-        <v>0.000867</v>
+        <v>86.7</v>
       </c>
       <c r="E90" t="n">
-        <v>0.000245</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="91">
@@ -1978,16 +1978,16 @@
         <v>1989</v>
       </c>
       <c r="B91" t="n">
-        <v>0.000498</v>
+        <v>49.8</v>
       </c>
       <c r="C91" t="n">
-        <v>0.000274</v>
+        <v>27.4</v>
       </c>
       <c r="D91" t="n">
-        <v>0.0008590000000000001</v>
+        <v>85.90000000000001</v>
       </c>
       <c r="E91" t="n">
-        <v>0.000241</v>
+        <v>24.1</v>
       </c>
     </row>
     <row r="92">
@@ -1995,16 +1995,16 @@
         <v>1990</v>
       </c>
       <c r="B92" t="n">
-        <v>0.000468</v>
+        <v>46.8</v>
       </c>
       <c r="C92" t="n">
-        <v>0.00026</v>
+        <v>26</v>
       </c>
       <c r="D92" t="n">
-        <v>0.000879</v>
+        <v>87.90000000000001</v>
       </c>
       <c r="E92" t="n">
-        <v>0.000222</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="93">
@@ -2012,16 +2012,16 @@
         <v>1991</v>
       </c>
       <c r="B93" t="n">
-        <v>0.000474</v>
+        <v>47.4</v>
       </c>
       <c r="C93" t="n">
-        <v>0.000256</v>
+        <v>25.6</v>
       </c>
       <c r="D93" t="n">
-        <v>0.000887</v>
+        <v>88.7</v>
       </c>
       <c r="E93" t="n">
-        <v>0.000215</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="94">
@@ -2029,16 +2029,16 @@
         <v>1992</v>
       </c>
       <c r="B94" t="n">
-        <v>0.000435</v>
+        <v>43.5</v>
       </c>
       <c r="C94" t="n">
-        <v>0.000244</v>
+        <v>24.4</v>
       </c>
       <c r="D94" t="n">
-        <v>0.0008359999999999999</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="E94" t="n">
-        <v>0.000203</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="95">
@@ -2046,16 +2046,16 @@
         <v>1993</v>
       </c>
       <c r="B95" t="n">
-        <v>0.000446</v>
+        <v>44.6</v>
       </c>
       <c r="C95" t="n">
-        <v>0.000253</v>
+        <v>25.3</v>
       </c>
       <c r="D95" t="n">
-        <v>0.0008579999999999999</v>
+        <v>85.8</v>
       </c>
       <c r="E95" t="n">
-        <v>0.00021</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96">
@@ -2063,16 +2063,16 @@
         <v>1994</v>
       </c>
       <c r="B96" t="n">
-        <v>0.000427</v>
+        <v>42.7</v>
       </c>
       <c r="C96" t="n">
-        <v>0.000248</v>
+        <v>24.8</v>
       </c>
       <c r="D96" t="n">
-        <v>0.000855</v>
+        <v>85.5</v>
       </c>
       <c r="E96" t="n">
-        <v>0.000197</v>
+        <v>19.7</v>
       </c>
     </row>
     <row r="97">
@@ -2080,16 +2080,16 @@
         <v>1995</v>
       </c>
       <c r="B97" t="n">
-        <v>0.000404</v>
+        <v>40.4</v>
       </c>
       <c r="C97" t="n">
-        <v>0.000251</v>
+        <v>25.1</v>
       </c>
       <c r="D97" t="n">
-        <v>0.0008209999999999999</v>
+        <v>82.09999999999999</v>
       </c>
       <c r="E97" t="n">
-        <v>0.000194</v>
+        <v>19.4</v>
       </c>
     </row>
     <row r="98">
@@ -2097,16 +2097,16 @@
         <v>1996</v>
       </c>
       <c r="B98" t="n">
-        <v>0.00038</v>
+        <v>38</v>
       </c>
       <c r="C98" t="n">
-        <v>0.000234</v>
+        <v>23.4</v>
       </c>
       <c r="D98" t="n">
-        <v>0.000775</v>
+        <v>77.5</v>
       </c>
       <c r="E98" t="n">
-        <v>0.00019</v>
+        <v>19</v>
       </c>
     </row>
     <row r="99">
@@ -2114,16 +2114,16 @@
         <v>1997</v>
       </c>
       <c r="B99" t="n">
-        <v>0.000355</v>
+        <v>35.5</v>
       </c>
       <c r="C99" t="n">
-        <v>0.000225</v>
+        <v>22.5</v>
       </c>
       <c r="D99" t="n">
-        <v>0.0007359999999999999</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="E99" t="n">
-        <v>0.00018</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100">
@@ -2131,16 +2131,16 @@
         <v>1998</v>
       </c>
       <c r="B100" t="n">
-        <v>0.000341</v>
+        <v>34.1</v>
       </c>
       <c r="C100" t="n">
-        <v>0.000215</v>
+        <v>21.5</v>
       </c>
       <c r="D100" t="n">
-        <v>0.000695</v>
+        <v>69.5</v>
       </c>
       <c r="E100" t="n">
-        <v>0.000172</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="101">
@@ -2148,16 +2148,16 @@
         <v>1999</v>
       </c>
       <c r="B101" t="n">
-        <v>0.000342</v>
+        <v>34.2</v>
       </c>
       <c r="C101" t="n">
-        <v>0.000204</v>
+        <v>20.4</v>
       </c>
       <c r="D101" t="n">
-        <v>0.000686</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="E101" t="n">
-        <v>0.000169</v>
+        <v>16.9</v>
       </c>
     </row>
     <row r="102">
@@ -2165,16 +2165,16 @@
         <v>2000</v>
       </c>
       <c r="B102" t="n">
-        <v>0.000324</v>
+        <v>32.4</v>
       </c>
       <c r="C102" t="n">
-        <v>0.000203</v>
+        <v>20.3</v>
       </c>
       <c r="D102" t="n">
-        <v>0.0006709999999999999</v>
+        <v>67.09999999999999</v>
       </c>
       <c r="E102" t="n">
-        <v>0.000158</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="103">
@@ -2182,16 +2182,16 @@
         <v>2001</v>
       </c>
       <c r="B103" t="n">
-        <v>0.000334</v>
+        <v>33.4</v>
       </c>
       <c r="C103" t="n">
-        <v>0.000191</v>
+        <v>19.1</v>
       </c>
       <c r="D103" t="n">
-        <v>0.000663</v>
+        <v>66.3</v>
       </c>
       <c r="E103" t="n">
-        <v>0.000153</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="104">
@@ -2199,16 +2199,16 @@
         <v>2002</v>
       </c>
       <c r="B104" t="n">
-        <v>0.000314</v>
+        <v>31.4</v>
       </c>
       <c r="C104" t="n">
-        <v>0.000194</v>
+        <v>19.4</v>
       </c>
       <c r="D104" t="n">
-        <v>0.00067</v>
+        <v>67</v>
       </c>
       <c r="E104" t="n">
-        <v>0.000152</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="105">
@@ -2216,16 +2216,16 @@
         <v>2003</v>
       </c>
       <c r="B105" t="n">
-        <v>0.000318</v>
+        <v>31.8</v>
       </c>
       <c r="C105" t="n">
-        <v>0.000189</v>
+        <v>18.9</v>
       </c>
       <c r="D105" t="n">
-        <v>0.0006540000000000001</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="E105" t="n">
-        <v>0.000148</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="106">
@@ -2233,16 +2233,16 @@
         <v>2004</v>
       </c>
       <c r="B106" t="n">
-        <v>0.000303</v>
+        <v>30.3</v>
       </c>
       <c r="C106" t="n">
-        <v>0.000184</v>
+        <v>18.4</v>
       </c>
       <c r="D106" t="n">
-        <v>0.0006490000000000001</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="E106" t="n">
-        <v>0.000148</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="107">
@@ -2250,16 +2250,16 @@
         <v>2005</v>
       </c>
       <c r="B107" t="n">
-        <v>0.000299</v>
+        <v>29.9</v>
       </c>
       <c r="C107" t="n">
-        <v>0.000177</v>
+        <v>17.7</v>
       </c>
       <c r="D107" t="n">
-        <v>0.000638</v>
+        <v>63.8</v>
       </c>
       <c r="E107" t="n">
-        <v>0.000146</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="108">
@@ -2267,16 +2267,16 @@
         <v>2006</v>
       </c>
       <c r="B108" t="n">
-        <v>0.000291</v>
+        <v>29.1</v>
       </c>
       <c r="C108" t="n">
-        <v>0.000162</v>
+        <v>16.2</v>
       </c>
       <c r="D108" t="n">
-        <v>0.00063</v>
+        <v>63</v>
       </c>
       <c r="E108" t="n">
-        <v>0.00014</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109">
@@ -2284,16 +2284,16 @@
         <v>2007</v>
       </c>
       <c r="B109" t="n">
-        <v>0.000294</v>
+        <v>29.4</v>
       </c>
       <c r="C109" t="n">
-        <v>0.000165</v>
+        <v>16.5</v>
       </c>
       <c r="D109" t="n">
-        <v>0.000603</v>
+        <v>60.3</v>
       </c>
       <c r="E109" t="n">
-        <v>0.000138</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="110">
@@ -2301,16 +2301,16 @@
         <v>2008</v>
       </c>
       <c r="B110" t="n">
-        <v>0.000293</v>
+        <v>29.3</v>
       </c>
       <c r="C110" t="n">
-        <v>0.000152</v>
+        <v>15.2</v>
       </c>
       <c r="D110" t="n">
-        <v>0.000559</v>
+        <v>55.9</v>
       </c>
       <c r="E110" t="n">
-        <v>0.000126</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="111">
@@ -2318,16 +2318,16 @@
         <v>2009</v>
       </c>
       <c r="B111" t="n">
-        <v>0.000274</v>
+        <v>27.4</v>
       </c>
       <c r="C111" t="n">
-        <v>0.000151</v>
+        <v>15.1</v>
       </c>
       <c r="D111" t="n">
-        <v>0.000519</v>
+        <v>51.9</v>
       </c>
       <c r="E111" t="n">
-        <v>0.000125</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="112">
@@ -2335,16 +2335,16 @@
         <v>2010</v>
       </c>
       <c r="B112" t="n">
-        <v>0.000265</v>
+        <v>26.5</v>
       </c>
       <c r="C112" t="n">
-        <v>0.000143</v>
+        <v>14.3</v>
       </c>
       <c r="D112" t="n">
-        <v>0.000494</v>
+        <v>49.4</v>
       </c>
       <c r="E112" t="n">
-        <v>0.000115</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="113">
@@ -2352,16 +2352,16 @@
         <v>2011</v>
       </c>
       <c r="B113" t="n">
-        <v>0.000263</v>
+        <v>26.3</v>
       </c>
       <c r="C113" t="n">
-        <v>0.000142</v>
+        <v>14.2</v>
       </c>
       <c r="D113" t="n">
-        <v>0.000489</v>
+        <v>48.9</v>
       </c>
       <c r="E113" t="n">
-        <v>0.000121</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="114">
@@ -2369,16 +2369,16 @@
         <v>2012</v>
       </c>
       <c r="B114" t="n">
-        <v>0.000263</v>
+        <v>26.3</v>
       </c>
       <c r="C114" t="n">
-        <v>0.000139</v>
+        <v>13.9</v>
       </c>
       <c r="D114" t="n">
-        <v>0.000472</v>
+        <v>47.2</v>
       </c>
       <c r="E114" t="n">
-        <v>0.000114</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="115">
@@ -2386,16 +2386,16 @@
         <v>2013</v>
       </c>
       <c r="B115" t="n">
-        <v>0.000255</v>
+        <v>25.5</v>
       </c>
       <c r="C115" t="n">
-        <v>0.000141</v>
+        <v>14.1</v>
       </c>
       <c r="D115" t="n">
-        <v>0.000448</v>
+        <v>44.8</v>
       </c>
       <c r="E115" t="n">
-        <v>0.000118</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="116">
@@ -2403,16 +2403,16 @@
         <v>2014</v>
       </c>
       <c r="B116" t="n">
-        <v>0.00024</v>
+        <v>24</v>
       </c>
       <c r="C116" t="n">
-        <v>0.00014</v>
+        <v>14</v>
       </c>
       <c r="D116" t="n">
-        <v>0.000455</v>
+        <v>45.5</v>
       </c>
       <c r="E116" t="n">
-        <v>0.000115</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="117">
@@ -2420,16 +2420,16 @@
         <v>2015</v>
       </c>
       <c r="B117" t="n">
-        <v>0.000249</v>
+        <v>24.9</v>
       </c>
       <c r="C117" t="n">
-        <v>0.000146</v>
+        <v>14.6</v>
       </c>
       <c r="D117" t="n">
-        <v>0.000483</v>
+        <v>48.3</v>
       </c>
       <c r="E117" t="n">
-        <v>0.000117</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="118">
@@ -2437,16 +2437,16 @@
         <v>2016</v>
       </c>
       <c r="B118" t="n">
-        <v>0.000253</v>
+        <v>25.3</v>
       </c>
       <c r="C118" t="n">
-        <v>0.000146</v>
+        <v>14.6</v>
       </c>
       <c r="D118" t="n">
-        <v>0.000512</v>
+        <v>51.2</v>
       </c>
       <c r="E118" t="n">
-        <v>0.000122</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="119">
@@ -2454,16 +2454,16 @@
         <v>2017</v>
       </c>
       <c r="B119" t="n">
-        <v>0.000243</v>
+        <v>24.3</v>
       </c>
       <c r="C119" t="n">
-        <v>0.000155</v>
+        <v>15.5</v>
       </c>
       <c r="D119" t="n">
-        <v>0.000515</v>
+        <v>51.5</v>
       </c>
       <c r="E119" t="n">
-        <v>0.000116</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="120">
@@ -2471,16 +2471,16 @@
         <v>2018</v>
       </c>
       <c r="B120" t="n">
-        <v>0.00024</v>
+        <v>24</v>
       </c>
       <c r="C120" t="n">
-        <v>0.000149</v>
+        <v>14.9</v>
       </c>
       <c r="D120" t="n">
-        <v>0.000492</v>
+        <v>49.2</v>
       </c>
       <c r="E120" t="n">
-        <v>0.000115</v>
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>